<commit_message>
Add file for archived results on old small data
</commit_message>
<xml_diff>
--- a/Ideal Result.xlsx
+++ b/Ideal Result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\avanish\dev\Denave\NERComparators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F6273D-CBD2-4711-B1C7-69F2A5C008F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73D9810-D4A6-40B5-96FF-1613E2B5BAD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -364,6 +364,1383 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IN" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Accuracy that matters</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IN">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Org Correct</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet2!$B$1:$L$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="11"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Small</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Medium</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Large</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Fast</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Large</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>ontonotes</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>small</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>on-fast</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>on-large</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>fast</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>small</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Spacy</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Flair</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Stanza</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Spark</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$3:$L$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8847-4CD1-8E4E-D746FA52166F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Org Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet2!$B$1:$L$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="11"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Small</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Medium</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Large</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Fast</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Large</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>ontonotes</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>small</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>on-fast</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>on-large</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>fast</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>small</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Spacy</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Flair</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Stanza</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Spark</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$4:$L$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>38.095238095238095</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.303370786516851</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50.96153846153846</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53.097345132743364</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>57.264957264957268</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75.555555555555557</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>52.252252252252255</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>62.365591397849464</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80.681818181818187</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55.752212389380531</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>75.555555555555557</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8847-4CD1-8E4E-D746FA52166F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Person Correct</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet2!$B$1:$L$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="11"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Small</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Medium</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Large</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Fast</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Large</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>ontonotes</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>small</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>on-fast</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>on-large</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>fast</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>small</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Spacy</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Flair</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Stanza</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Spark</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$5:$L$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8847-4CD1-8E4E-D746FA52166F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Person Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet2!$B$1:$L$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="11"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Small</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Medium</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Large</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Fast</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Large</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>ontonotes</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>small</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>on-fast</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>on-large</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>fast</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>small</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Spacy</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Flair</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Stanza</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Spark</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$6:$L$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>56.521739130434781</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>84.782608695652172</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>91.666666666666671</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>96.969696969696969</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>91.489361702127653</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8847-4CD1-8E4E-D746FA52166F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2135879680"/>
+        <c:axId val="2135886752"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2135879680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2135886752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2135886752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2135879680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B293C4D-9088-48AF-B131-6D1E7A329039}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1168,7 +2545,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="E11" sqref="E11:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1234,252 +2611,252 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B3">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>51</v>
+      </c>
+      <c r="D3">
+        <v>53</v>
+      </c>
+      <c r="E3">
+        <v>60</v>
+      </c>
+      <c r="F3">
+        <v>67</v>
+      </c>
+      <c r="G3">
+        <v>68</v>
+      </c>
+      <c r="H3">
+        <v>58</v>
+      </c>
+      <c r="I3">
+        <v>58</v>
+      </c>
+      <c r="J3">
+        <v>71</v>
+      </c>
+      <c r="K3">
         <v>63</v>
       </c>
-      <c r="C3">
-        <v>89</v>
-      </c>
-      <c r="D3">
-        <v>104</v>
-      </c>
-      <c r="E3">
-        <v>113</v>
-      </c>
-      <c r="F3">
-        <v>117</v>
-      </c>
-      <c r="G3">
-        <v>90</v>
-      </c>
-      <c r="H3">
-        <v>111</v>
-      </c>
-      <c r="I3">
-        <v>93</v>
-      </c>
-      <c r="J3">
-        <v>88</v>
-      </c>
-      <c r="K3">
-        <v>113</v>
-      </c>
       <c r="L3">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="B4">
-        <v>24</v>
+        <f>(B$3*100)/B$8</f>
+        <v>38.095238095238095</v>
       </c>
       <c r="C4">
-        <v>51</v>
+        <f>(C$3*100)/C$8</f>
+        <v>57.303370786516851</v>
       </c>
       <c r="D4">
-        <v>53</v>
+        <f>(D$3*100)/D$8</f>
+        <v>50.96153846153846</v>
       </c>
       <c r="E4">
-        <v>60</v>
+        <f>(E$3*100)/E$8</f>
+        <v>53.097345132743364</v>
       </c>
       <c r="F4">
-        <v>67</v>
+        <f>(F$3*100)/F$8</f>
+        <v>57.264957264957268</v>
       </c>
       <c r="G4">
-        <v>68</v>
+        <f>(G$3*100)/G$8</f>
+        <v>75.555555555555557</v>
       </c>
       <c r="H4">
-        <v>58</v>
+        <f>(H$3*100)/H$8</f>
+        <v>52.252252252252255</v>
       </c>
       <c r="I4">
-        <v>58</v>
+        <f>(I$3*100)/I$8</f>
+        <v>62.365591397849464</v>
       </c>
       <c r="J4">
-        <v>71</v>
+        <f>(J$3*100)/J$8</f>
+        <v>80.681818181818187</v>
       </c>
       <c r="K4">
-        <v>63</v>
+        <f>(K$3*100)/K$8</f>
+        <v>55.752212389380531</v>
       </c>
       <c r="L4">
-        <v>34</v>
+        <f>(L$3*100)/L$8</f>
+        <v>75.555555555555557</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B5">
-        <f>(B$4*100)/B$3</f>
-        <v>38.095238095238095</v>
+        <v>26</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:L5" si="0">(C$4*100)/C$3</f>
-        <v>57.303370786516851</v>
+        <v>39</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>50.96153846153846</v>
+        <v>33</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
-        <v>53.097345132743364</v>
+        <v>31</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
-        <v>57.264957264957268</v>
+        <v>49</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
-        <v>75.555555555555557</v>
+        <v>39</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
-        <v>52.252252252252255</v>
+        <v>30</v>
       </c>
       <c r="I5">
-        <f t="shared" si="0"/>
-        <v>62.365591397849464</v>
+        <v>36</v>
       </c>
       <c r="J5">
-        <f t="shared" si="0"/>
-        <v>80.681818181818187</v>
+        <v>47</v>
       </c>
       <c r="K5">
-        <f t="shared" si="0"/>
-        <v>55.752212389380531</v>
+        <v>32</v>
       </c>
       <c r="L5">
-        <f t="shared" si="0"/>
-        <v>75.555555555555557</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="B6">
-        <v>46</v>
+        <f>(B$5*100)/B$9</f>
+        <v>56.521739130434781</v>
       </c>
       <c r="C6">
-        <v>46</v>
+        <f>(C$5*100)/C$9</f>
+        <v>84.782608695652172</v>
       </c>
       <c r="D6">
-        <v>36</v>
+        <f>(D$5*100)/D$9</f>
+        <v>91.666666666666671</v>
       </c>
       <c r="E6">
-        <v>31</v>
+        <f>(E$5*100)/E$9</f>
+        <v>100</v>
       </c>
       <c r="F6">
-        <v>49</v>
+        <f>(F$5*100)/F$9</f>
+        <v>100</v>
       </c>
       <c r="G6">
-        <v>40</v>
+        <f>(G$5*100)/G$9</f>
+        <v>97.5</v>
       </c>
       <c r="H6">
-        <v>30</v>
+        <f>(H$5*100)/H$9</f>
+        <v>100</v>
       </c>
       <c r="I6">
-        <v>36</v>
+        <f>(I$5*100)/I$9</f>
+        <v>100</v>
       </c>
       <c r="J6">
-        <v>50</v>
+        <f>(J$5*100)/J$9</f>
+        <v>94</v>
       </c>
       <c r="K6">
-        <v>33</v>
+        <f>(K$5*100)/K$9</f>
+        <v>96.969696969696969</v>
       </c>
       <c r="L6">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7">
-        <v>26</v>
-      </c>
-      <c r="C7">
-        <v>39</v>
-      </c>
-      <c r="D7">
-        <v>33</v>
-      </c>
-      <c r="E7">
-        <v>31</v>
-      </c>
-      <c r="F7">
-        <v>49</v>
-      </c>
-      <c r="G7">
-        <v>39</v>
-      </c>
-      <c r="H7">
-        <v>30</v>
-      </c>
-      <c r="I7">
-        <v>36</v>
-      </c>
-      <c r="J7">
-        <v>47</v>
-      </c>
-      <c r="K7">
-        <v>32</v>
-      </c>
-      <c r="L7">
-        <v>43</v>
+        <f>(L$5*100)/L$9</f>
+        <v>91.489361702127653</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B8">
-        <f>(B$7*100)/B$6</f>
-        <v>56.521739130434781</v>
+        <v>63</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C8:L8" si="1">(C$7*100)/C$6</f>
-        <v>84.782608695652172</v>
+        <v>89</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
-        <v>91.666666666666671</v>
+        <v>104</v>
       </c>
       <c r="E8">
-        <f t="shared" si="1"/>
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
-        <v>97.5</v>
+        <v>90</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="I8">
-        <f t="shared" si="1"/>
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="J8">
-        <f t="shared" si="1"/>
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="K8">
-        <f t="shared" si="1"/>
-        <v>96.969696969696969</v>
+        <v>113</v>
       </c>
       <c r="L8">
-        <f t="shared" si="1"/>
-        <v>91.489361702127653</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9">
+        <v>46</v>
+      </c>
+      <c r="C9">
+        <v>46</v>
+      </c>
+      <c r="D9">
+        <v>36</v>
+      </c>
+      <c r="E9">
+        <v>31</v>
+      </c>
+      <c r="F9">
+        <v>49</v>
+      </c>
+      <c r="G9">
+        <v>40</v>
+      </c>
+      <c r="H9">
+        <v>30</v>
+      </c>
+      <c r="I9">
+        <v>36</v>
+      </c>
+      <c r="J9">
+        <v>50</v>
+      </c>
+      <c r="K9">
+        <v>33</v>
+      </c>
+      <c r="L9">
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -1604,5 +2981,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>